<commit_message>
instructions: recommend ISO 8601 for dates + some minor edits
</commit_message>
<xml_diff>
--- a/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
+++ b/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\example_submission_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Data-Notes\BLE-Practices\metadata_templates\canon\example_submission_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" activeTab="8"/>
+    <workbookView xWindow="930" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="335">
   <si>
     <t>StorageType</t>
   </si>
@@ -1036,6 +1036,12 @@
   </si>
   <si>
     <t>Station is not part of regional survey and so does not get a station identifier</t>
+  </si>
+  <si>
+    <t>Update Frequency</t>
+  </si>
+  <si>
+    <t>notPlanned</t>
   </si>
 </sst>
 </file>
@@ -2226,11 +2232,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,7 +2256,7 @@
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2293,8 +2299,11 @@
       <c r="N1" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="D2" s="6" t="s">
         <v>195</v>
       </c>
@@ -2320,8 +2329,11 @@
       <c r="N2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2531,7 +2543,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list">
           <x14:formula1>
-            <xm:f>'[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
+            <xm:f>'\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\example_submission_package\[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -2972,7 +2984,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid">
           <x14:formula1>
-            <xm:f>'[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
+            <xm:f>'\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\example_submission_package\[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E21</xm:sqref>
         </x14:dataValidation>
@@ -4541,10 +4553,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add pubs to example
</commit_message>
<xml_diff>
--- a/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
+++ b/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Data-Notes\BLE-Practices\metadata_templates\canon\example_submission_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\canon\example_submission_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" activeTab="1"/>
+    <workbookView xWindow="2376" yWindow="468" windowWidth="25608" windowHeight="14232" tabRatio="913" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -22,10 +22,11 @@
     <sheet name="Attribute Codes" sheetId="4" r:id="rId8"/>
     <sheet name="Attribute Missing Values" sheetId="25" r:id="rId9"/>
     <sheet name="Taxonomic" sheetId="26" state="hidden" r:id="rId10"/>
-    <sheet name="lookup_tables" sheetId="24" r:id="rId11"/>
+    <sheet name="Related Pubs" sheetId="28" r:id="rId11"/>
+    <sheet name="lookup_tables" sheetId="24" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="341">
   <si>
     <t>StorageType</t>
   </si>
@@ -1042,6 +1043,24 @@
   </si>
   <si>
     <t>notPlanned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication </t>
+  </si>
+  <si>
+    <t>Relationship to Dataset</t>
+  </si>
+  <si>
+    <t>Publication-Data Relationships</t>
+  </si>
+  <si>
+    <t>data cites pub (method/idea)</t>
+  </si>
+  <si>
+    <t>pub uses this data</t>
+  </si>
+  <si>
+    <t>pub is data paper about data</t>
   </si>
 </sst>
 </file>
@@ -1712,9 +1731,9 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1729,7 +1748,7 @@
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="27" t="s">
         <v>194</v>
@@ -1746,7 +1765,7 @@
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="27" t="s">
         <v>193</v>
@@ -1763,7 +1782,7 @@
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -1792,14 +1811,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -1820,22 +1839,68 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="64.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="info to ID the publication: can be a citation (any format), a DOI, a link" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="indicate the relationship between the dataset and the publication" sqref="B1"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[metadata_template.xlsx]lookup_tables!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B50</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" customWidth="1"/>
+    <col min="4" max="4" width="44.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="64.5546875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>86</v>
       </c>
@@ -1850,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>54</v>
       </c>
@@ -1873,7 +1938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
@@ -1896,7 +1961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>57</v>
       </c>
@@ -1916,7 +1981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
@@ -1936,7 +2001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>77</v>
       </c>
@@ -1959,7 +2024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>79</v>
       </c>
@@ -1977,7 +2042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>82</v>
       </c>
@@ -1995,7 +2060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F9" s="14" t="s">
         <v>94</v>
       </c>
@@ -2003,7 +2068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -2026,7 +2091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2043,7 +2108,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2060,7 +2125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2075,7 +2140,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2090,7 +2155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
         <v>30</v>
       </c>
@@ -2102,7 +2167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
@@ -2112,7 +2177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>6</v>
       </c>
@@ -2122,13 +2187,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
       <c r="I18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>104</v>
       </c>
@@ -2140,7 +2205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>105</v>
       </c>
@@ -2157,7 +2222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -2174,7 +2239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -2185,7 +2250,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -2196,7 +2261,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2207,7 +2272,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2216,6 +2281,26 @@
       </c>
       <c r="C25" s="6" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2234,29 +2319,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2303,7 +2388,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D2" s="6" t="s">
         <v>195</v>
       </c>
@@ -2333,7 +2418,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2383,24 +2468,24 @@
       <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
-    <col min="10" max="15" width="8.85546875" style="1"/>
-    <col min="16" max="16" width="8.85546875" style="3"/>
-    <col min="17" max="17" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="13.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="1" customWidth="1"/>
+    <col min="10" max="15" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="8.88671875" style="3"/>
+    <col min="17" max="17" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2465,7 +2550,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2563,21 +2648,21 @@
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="9.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="6"/>
     <col min="7" max="7" width="40" style="6" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="80.28515625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="36.6640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="80.33203125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2603,7 +2688,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>211</v>
       </c>
@@ -2627,7 +2712,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>212</v>
       </c>
@@ -2651,7 +2736,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>213</v>
       </c>
@@ -2675,7 +2760,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>214</v>
       </c>
@@ -2699,7 +2784,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>215</v>
       </c>
@@ -2721,7 +2806,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>216</v>
       </c>
@@ -2743,7 +2828,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>217</v>
       </c>
@@ -2758,7 +2843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>218</v>
       </c>
@@ -2773,7 +2858,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>219</v>
       </c>
@@ -2788,7 +2873,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>220</v>
       </c>
@@ -2803,7 +2888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>221</v>
       </c>
@@ -2818,7 +2903,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>222</v>
       </c>
@@ -2833,7 +2918,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>223</v>
       </c>
@@ -2848,7 +2933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>224</v>
       </c>
@@ -2863,7 +2948,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>225</v>
       </c>
@@ -2878,7 +2963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>226</v>
       </c>
@@ -2893,7 +2978,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>227</v>
       </c>
@@ -2908,7 +2993,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>228</v>
       </c>
@@ -2923,7 +3008,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>229</v>
       </c>
@@ -2938,7 +3023,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>230</v>
       </c>
@@ -3003,27 +3088,27 @@
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="24.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="24.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3076,7 +3161,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>131</v>
       </c>
@@ -3095,21 +3180,21 @@
       <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="8" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3141,7 +3226,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2"/>
       <c r="C2" s="6" t="s">
         <v>231</v>
@@ -3160,7 +3245,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3"/>
       <c r="C3" s="6" t="s">
         <v>235</v>
@@ -3179,7 +3264,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C4" s="6" t="s">
         <v>238</v>
       </c>
@@ -3197,7 +3282,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
         <v>241</v>
       </c>
@@ -3234,29 +3319,29 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="1"/>
+    <col min="17" max="17" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -3309,7 +3394,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -3327,7 +3412,7 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
     </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -3345,7 +3430,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -3363,7 +3448,7 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -3381,7 +3466,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -3399,7 +3484,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -3423,7 +3508,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -3447,7 +3532,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -3465,7 +3550,7 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -3483,7 +3568,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>231</v>
       </c>
@@ -3501,7 +3586,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>231</v>
       </c>
@@ -3525,7 +3610,7 @@
       </c>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>231</v>
       </c>
@@ -3549,7 +3634,7 @@
       </c>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>231</v>
       </c>
@@ -3571,7 +3656,7 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>231</v>
       </c>
@@ -3595,7 +3680,7 @@
       </c>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>231</v>
       </c>
@@ -3619,7 +3704,7 @@
       </c>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>231</v>
       </c>
@@ -3641,7 +3726,7 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" ht="72" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>231</v>
       </c>
@@ -3663,7 +3748,7 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>231</v>
       </c>
@@ -3685,7 +3770,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>231</v>
       </c>
@@ -3703,7 +3788,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>235</v>
       </c>
@@ -3721,7 +3806,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>235</v>
       </c>
@@ -3739,7 +3824,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>235</v>
       </c>
@@ -3763,7 +3848,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>235</v>
       </c>
@@ -3787,7 +3872,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>235</v>
       </c>
@@ -3805,7 +3890,7 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>235</v>
       </c>
@@ -3827,7 +3912,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>235</v>
       </c>
@@ -3851,7 +3936,7 @@
       </c>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>235</v>
       </c>
@@ -3873,7 +3958,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>238</v>
       </c>
@@ -3897,7 +3982,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>238</v>
       </c>
@@ -3921,7 +4006,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>238</v>
       </c>
@@ -3939,7 +4024,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>238</v>
       </c>
@@ -3957,7 +4042,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>238</v>
       </c>
@@ -3975,7 +4060,7 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="2:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>238</v>
       </c>
@@ -3997,7 +4082,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>238</v>
       </c>
@@ -4021,7 +4106,7 @@
       </c>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>238</v>
       </c>
@@ -4043,7 +4128,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>238</v>
       </c>
@@ -4067,7 +4152,7 @@
       </c>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>238</v>
       </c>
@@ -4091,7 +4176,7 @@
       </c>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>241</v>
       </c>
@@ -4115,7 +4200,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>241</v>
       </c>
@@ -4139,7 +4224,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>241</v>
       </c>
@@ -4157,7 +4242,7 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>241</v>
       </c>
@@ -4175,7 +4260,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>241</v>
       </c>
@@ -4199,7 +4284,7 @@
       </c>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" ht="72" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>241</v>
       </c>
@@ -4221,7 +4306,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="2:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>241</v>
       </c>
@@ -4243,7 +4328,7 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="6"/>
     </row>
   </sheetData>
@@ -4317,15 +4402,15 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4342,7 +4427,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -4356,7 +4441,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -4370,7 +4455,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4384,7 +4469,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -4398,7 +4483,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -4412,7 +4497,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -4426,7 +4511,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -4440,7 +4525,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -4454,7 +4539,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -4468,7 +4553,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>231</v>
       </c>
@@ -4482,7 +4567,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>231</v>
       </c>
@@ -4496,7 +4581,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>231</v>
       </c>
@@ -4559,16 +4644,16 @@
       <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4585,7 +4670,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -4599,7 +4684,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -4613,7 +4698,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4627,7 +4712,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -4641,7 +4726,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -4655,7 +4740,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -4669,7 +4754,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -4683,7 +4768,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -4697,7 +4782,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -4711,7 +4796,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>235</v>
       </c>
@@ -4725,7 +4810,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>235</v>
       </c>
@@ -4739,7 +4824,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>235</v>
       </c>
@@ -4753,7 +4838,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>235</v>
       </c>
@@ -4767,7 +4852,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>235</v>
       </c>
@@ -4781,7 +4866,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>235</v>
       </c>
@@ -4795,7 +4880,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>238</v>
       </c>
@@ -4809,7 +4894,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>238</v>
       </c>
@@ -4823,7 +4908,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>238</v>
       </c>
@@ -4837,7 +4922,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>238</v>
       </c>
@@ -4851,7 +4936,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>241</v>
       </c>
@@ -4865,7 +4950,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>241</v>
       </c>

</xml_diff>

<commit_message>
Add two columns to dataset tab in example to match template
</commit_message>
<xml_diff>
--- a/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
+++ b/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Data-Notes\BLE-Practices\metadata_templates\canon\example_submission_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whiteatl\Documents\ble-metadata-template\example_submission_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDC5227-2B70-4AD0-9E95-1AB1EE4D739F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3816" yWindow="468" windowWidth="25608" windowHeight="14232" tabRatio="913" activeTab="10"/>
+    <workbookView xWindow="3810" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -27,9 +28,8 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="346">
   <si>
     <t>StorageType</t>
   </si>
@@ -1065,12 +1065,24 @@
   </si>
   <si>
     <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2020GB006552</t>
+  </si>
+  <si>
+    <t>Core Program?</t>
+  </si>
+  <si>
+    <t>Primarily funded by BLE LTER?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1416,7 +1428,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1461,19 +1473,6 @@
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="lookup_tables"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1741,16 +1740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1765,7 +1762,7 @@
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="27" t="s">
         <v>194</v>
@@ -1782,7 +1779,7 @@
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="27" t="s">
         <v>193</v>
@@ -1799,7 +1796,7 @@
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -1821,21 +1818,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -1855,21 +1852,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>335</v>
       </c>
@@ -1877,7 +1874,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>341</v>
       </c>
@@ -1887,14 +1884,14 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="info to ID the publication: can be a citation (any format), a DOI, a link" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="indicate the relationship between the dataset and the publication" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="info to ID the publication: can be a citation (any format), a DOI, a link" sqref="A1" xr:uid="{00000000-0002-0000-0A00-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="indicate the relationship between the dataset and the publication" sqref="B1" xr:uid="{00000000-0002-0000-0A00-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$A$28:$A$30</xm:f>
           </x14:formula1>
@@ -1907,25 +1904,23 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="64.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="64.5703125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>86</v>
       </c>
@@ -1940,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>54</v>
       </c>
@@ -1963,7 +1958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
@@ -1986,7 +1981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>57</v>
       </c>
@@ -2006,7 +2001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
@@ -2026,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>77</v>
       </c>
@@ -2049,7 +2044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>79</v>
       </c>
@@ -2067,7 +2062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>82</v>
       </c>
@@ -2085,7 +2080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F9" s="14" t="s">
         <v>94</v>
       </c>
@@ -2093,7 +2088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -2116,7 +2111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2133,7 +2128,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2150,7 +2145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2165,7 +2160,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2180,7 +2175,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>30</v>
       </c>
@@ -2192,7 +2187,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
@@ -2202,7 +2197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>6</v>
       </c>
@@ -2212,13 +2207,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="I18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>104</v>
       </c>
@@ -2230,7 +2225,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>105</v>
       </c>
@@ -2247,7 +2242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -2264,7 +2259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -2275,7 +2270,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -2286,7 +2281,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2297,7 +2292,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2308,32 +2303,32 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>340</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -2341,32 +2336,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2412,8 +2410,14 @@
       <c r="O1" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="P1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="D2" s="6" t="s">
         <v>195</v>
       </c>
@@ -2442,8 +2446,14 @@
       <c r="O2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2453,26 +2463,32 @@
       <c r="N4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 15 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Send us a Word doc and enter file name here. See PDF for guidelines." sqref="E2:E4 H2:H4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Earliest date in dataset. Use YYYY-MM-DD or YYYY." sqref="I2:I4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latest date in dataset. Use YYYY-MM-DD or YYYY." sqref="J2:J4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CC0 or Creative Commons 0, a public domain license, is the license we use for our datasets. If you wish to use a different license, please discuss with the information managers." sqref="M2:M4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The timezone used for any date/time values supplied in this dataset." sqref="N2:N4"/>
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 15 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Send us a Word doc and enter file name here. See PDF for guidelines." sqref="E2:E4 H2:H4" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Earliest date in dataset. Use YYYY-MM-DD or YYYY." sqref="I2:I4" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latest date in dataset. Use YYYY-MM-DD or YYYY." sqref="J2:J4" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CC0 or Creative Commons 0, a public domain license, is the license we use for our datasets. If you wish to use a different license, please discuss with the information managers." sqref="M2:M4" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The timezone used for any date/time values supplied in this dataset." sqref="N2:N4" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Is this a BLE Core Program dataset?" sqref="P2" xr:uid="{45D80D48-DC92-448B-BE8A-5902A4656AE5}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Was this dataset primarly funded by BLE? If not, you'll need to provide the information manager with details about other projects funding this dataset." sqref="Q2" xr:uid="{0053398A-2209-4777-BEC2-C55F217D7B23}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value.">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value." xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$D$11:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>K2:K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="make sure we can locate this authority" prompt="The taxonomic authority to which you refer when determining taxonomic names in this dataset. The drop-down options are ITIS and WoRMS, commonly used in marine bio, or enter your own.">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="make sure we can locate this authority" prompt="The taxonomic authority to which you refer when determining taxonomic names in this dataset. The drop-down options are ITIS and WoRMS, commonly used in marine bio, or enter your own." xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$D$20:$D$21</xm:f>
           </x14:formula1>
@@ -2485,32 +2501,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" style="1" customWidth="1"/>
-    <col min="10" max="15" width="8.88671875" style="1"/>
-    <col min="16" max="16" width="8.88671875" style="3"/>
-    <col min="17" max="17" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.88671875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
+    <col min="10" max="15" width="8.85546875" style="1"/>
+    <col min="16" max="16" width="8.85546875" style="3"/>
+    <col min="17" max="17" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2575,7 +2591,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2628,30 +2644,30 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" sqref="C1"/>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Number all creators starting with 2." prompt="Analogous to authorship order in a publication. Per LTER best practices, BLE will be first creator to any BLE dataset, so number all creators starting with 2. _x000a__x000a_Leave blank for all other roles." sqref="D3:D4">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" sqref="C1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Number all creators starting with 2." prompt="Analogous to authorship order in a publication. Per LTER best practices, BLE will be first creator to any BLE dataset, so number all creators starting with 2. _x000a__x000a_Leave blank for all other roles." sqref="D3:D4" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORCID is a unique identifier system for researchers. Sign up at https://orcid.org. This person doesn't have an ORCID? Maybe encourage them to get one and fill out a profile? (Merely having an ORCID is no good without a nice profile.)" sqref="H3:H4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORCID is a unique identifier system for researchers. Sign up at https://orcid.org. This person doesn't have an ORCID? Maybe encourage them to get one and fill out a profile? (Merely having an ORCID is no good without a nice profile.)" sqref="H3:H4" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$F$3:$F$10</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" prompt="Include dataset creators, but also technicians and other personnel who contribute to and deserve acknowledgment for this dataset._x000a__x000a_Choose from a value in the drop down or enter your own value.">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" prompt="Include dataset creators, but also technicians and other personnel who contribute to and deserve acknowledgment for this dataset._x000a__x000a_Choose from a value in the drop down or enter your own value." xr:uid="{00000000-0002-0000-0200-000004000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$F$3:$F$10</xm:f>
           </x14:formula1>
           <xm:sqref>C3:C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" xr:uid="{00000000-0002-0000-0200-000005000000}">
           <x14:formula1>
             <xm:f>'\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\example_submission_package\[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
           </x14:formula1>
@@ -2664,30 +2680,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="6" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="9.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="6"/>
     <col min="7" max="7" width="40" style="6" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="80.33203125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="8" max="8" width="36.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="80.28515625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2713,7 +2729,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>211</v>
       </c>
@@ -2737,7 +2753,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>212</v>
       </c>
@@ -2761,7 +2777,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>213</v>
       </c>
@@ -2785,7 +2801,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>214</v>
       </c>
@@ -2809,7 +2825,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>215</v>
       </c>
@@ -2831,7 +2847,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>216</v>
       </c>
@@ -2853,7 +2869,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>217</v>
       </c>
@@ -2868,7 +2884,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>218</v>
       </c>
@@ -2883,7 +2899,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>219</v>
       </c>
@@ -2898,7 +2914,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>220</v>
       </c>
@@ -2913,7 +2929,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>221</v>
       </c>
@@ -2928,7 +2944,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>222</v>
       </c>
@@ -2943,7 +2959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>223</v>
       </c>
@@ -2958,7 +2974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>224</v>
       </c>
@@ -2973,7 +2989,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>225</v>
       </c>
@@ -2988,7 +3004,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>226</v>
       </c>
@@ -3003,7 +3019,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>227</v>
       </c>
@@ -3018,7 +3034,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>228</v>
       </c>
@@ -3033,7 +3049,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>229</v>
       </c>
@@ -3048,7 +3064,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>230</v>
       </c>
@@ -3065,34 +3081,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$C$11:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>E22:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$A$3:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>D5:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="We highly recommend choosing keywords from an existing keyword set, aka thesaurus. See the included table for links to preferred thesauri. _x000a__x000a_Choose from the drop-down menu. Choose &quot;none&quot; if the keyword did not come from any thesauri (not recommended!).">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="We highly recommend choosing keywords from an existing keyword set, aka thesaurus. See the included table for links to preferred thesauri. _x000a__x000a_Choose from the drop-down menu. Choose &quot;none&quot; if the keyword did not come from any thesauri (not recommended!)." xr:uid="{00000000-0002-0000-0300-000002000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$A$3:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid" xr:uid="{00000000-0002-0000-0300-000003000000}">
           <x14:formula1>
             <xm:f>'\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\example_submission_package\[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
           </x14:formula1>
@@ -3105,7 +3121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3113,27 +3129,27 @@
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="24.44140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3186,7 +3202,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>131</v>
       </c>
@@ -3197,29 +3213,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="8" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3251,7 +3267,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2" s="6" t="s">
         <v>231</v>
@@ -3270,7 +3286,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3" s="6" t="s">
         <v>235</v>
@@ -3289,7 +3305,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>238</v>
       </c>
@@ -3307,7 +3323,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>241</v>
       </c>
@@ -3327,7 +3343,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
@@ -3336,37 +3352,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -3419,7 +3435,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -3437,7 +3453,7 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
     </row>
-    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -3455,7 +3471,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -3473,7 +3489,7 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -3491,7 +3507,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -3509,7 +3525,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -3533,7 +3549,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -3557,7 +3573,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -3575,7 +3591,7 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -3593,7 +3609,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>231</v>
       </c>
@@ -3611,7 +3627,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>231</v>
       </c>
@@ -3635,7 +3651,7 @@
       </c>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>231</v>
       </c>
@@ -3659,7 +3675,7 @@
       </c>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>231</v>
       </c>
@@ -3681,7 +3697,7 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>231</v>
       </c>
@@ -3705,7 +3721,7 @@
       </c>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>231</v>
       </c>
@@ -3729,7 +3745,7 @@
       </c>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>231</v>
       </c>
@@ -3751,7 +3767,7 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="2:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" ht="75" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>231</v>
       </c>
@@ -3773,7 +3789,7 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="2:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>231</v>
       </c>
@@ -3795,7 +3811,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>231</v>
       </c>
@@ -3813,7 +3829,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>235</v>
       </c>
@@ -3831,7 +3847,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>235</v>
       </c>
@@ -3849,7 +3865,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>235</v>
       </c>
@@ -3873,7 +3889,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>235</v>
       </c>
@@ -3897,7 +3913,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>235</v>
       </c>
@@ -3915,7 +3931,7 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>235</v>
       </c>
@@ -3937,7 +3953,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>235</v>
       </c>
@@ -3961,7 +3977,7 @@
       </c>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>235</v>
       </c>
@@ -3983,7 +3999,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>238</v>
       </c>
@@ -4007,7 +4023,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>238</v>
       </c>
@@ -4031,7 +4047,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>238</v>
       </c>
@@ -4049,7 +4065,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>238</v>
       </c>
@@ -4067,7 +4083,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>238</v>
       </c>
@@ -4085,7 +4101,7 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>238</v>
       </c>
@@ -4107,7 +4123,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>238</v>
       </c>
@@ -4131,7 +4147,7 @@
       </c>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>238</v>
       </c>
@@ -4153,7 +4169,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>238</v>
       </c>
@@ -4177,7 +4193,7 @@
       </c>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>238</v>
       </c>
@@ -4201,7 +4217,7 @@
       </c>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>241</v>
       </c>
@@ -4225,7 +4241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>241</v>
       </c>
@@ -4249,7 +4265,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>241</v>
       </c>
@@ -4267,7 +4283,7 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>241</v>
       </c>
@@ -4285,7 +4301,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>241</v>
       </c>
@@ -4309,7 +4325,7 @@
       </c>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="2:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:17" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>241</v>
       </c>
@@ -4331,7 +4347,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="2:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:17" ht="60" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>241</v>
       </c>
@@ -4353,27 +4369,27 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter whole numbers numbering your columns" sqref="C101:C1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter whole numbers numbering your columns" sqref="C101:C1048576" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." sqref="C46:C49 C51:C100">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." sqref="C46:C49 C51:C100" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." sqref="N46:N100">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." sqref="N46:N100" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value." sqref="P46:Q100">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value." sqref="P46:Q100" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>ISNUMBER(P45)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value" sqref="N2:N45">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value" sqref="N2:N45" xr:uid="{00000000-0002-0000-0600-000004000000}">
       <formula1>ISNUMBER(N2)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value_x000a_" sqref="P2:Q45">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value_x000a_" sqref="P2:Q45" xr:uid="{00000000-0002-0000-0600-000005000000}">
       <formula1>ISNUMBER(P2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -4382,31 +4398,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from the four!" prompt="choose from four number types">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from the four!" prompt="choose from four number types" xr:uid="{00000000-0002-0000-0600-000006000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$A$11:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>O2:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" error="choose from the seven!" prompt="choose from the seven">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" error="choose from the seven!" prompt="choose from the seven" xr:uid="{00000000-0002-0000-0600-000007000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$B$11:$B$17</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I24 I29:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" xr:uid="{00000000-0002-0000-0600-000008000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$I$2:$I$21</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H24 H29:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;" xr:uid="{00000000-0002-0000-0600-000009000000}">
           <x14:formula1>
             <xm:f>Entities!$J$4:$J$30</xm:f>
           </x14:formula1>
           <xm:sqref>B51:B100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-00000A000000}">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$11</xm:f>
           </x14:formula1>
@@ -4419,23 +4435,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4452,7 +4468,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -4466,7 +4482,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -4480,7 +4496,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4494,7 +4510,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -4508,7 +4524,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -4522,7 +4538,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -4536,7 +4552,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -4550,7 +4566,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -4564,7 +4580,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -4578,7 +4594,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>231</v>
       </c>
@@ -4592,7 +4608,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>231</v>
       </c>
@@ -4606,7 +4622,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>231</v>
       </c>
@@ -4622,32 +4638,32 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact code as appears in data." sqref="D2:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Define this code (even if it seems self-explanatory)." sqref="E2:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact code as appears in data." sqref="D2:D4" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Define this code (even if it seems self-explanatory)." sqref="E2:E4" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that you have entered in the &quot;Attributes&quot; sheet">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that you have entered in the &quot;Attributes&quot; sheet" xr:uid="{00000000-0002-0000-0700-000002000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears in the &quot;Attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet.">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears in the &quot;Attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet." xr:uid="{00000000-0002-0000-0700-000003000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000004000000}">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B50</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;" xr:uid="{00000000-0002-0000-0700-000005000000}">
           <x14:formula1>
             <xm:f>Entities!$J$4:$J$30</xm:f>
           </x14:formula1>
@@ -4660,25 +4676,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4695,7 +4711,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -4709,7 +4725,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -4723,7 +4739,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4737,7 +4753,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -4751,7 +4767,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -4765,7 +4781,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -4779,7 +4795,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -4793,7 +4809,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -4807,7 +4823,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -4821,7 +4837,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>235</v>
       </c>
@@ -4835,7 +4851,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>235</v>
       </c>
@@ -4849,7 +4865,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>235</v>
       </c>
@@ -4863,7 +4879,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>235</v>
       </c>
@@ -4877,7 +4893,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>235</v>
       </c>
@@ -4891,7 +4907,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>235</v>
       </c>
@@ -4905,7 +4921,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>238</v>
       </c>
@@ -4919,7 +4935,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>238</v>
       </c>
@@ -4933,7 +4949,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>238</v>
       </c>
@@ -4947,7 +4963,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>238</v>
       </c>
@@ -4961,7 +4977,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>241</v>
       </c>
@@ -4975,7 +4991,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>241</v>
       </c>
@@ -4991,32 +5007,32 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact missing value code as appears in data." sqref="D2:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Why are missing values represented by this code missing? " sqref="E2:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact missing value code as appears in data." sqref="D2:D4" xr:uid="{00000000-0002-0000-0800-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Why are missing values represented by this code missing? " sqref="E2:E4" xr:uid="{00000000-0002-0000-0800-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name you have entered in the &quot;attributes&quot; sheet">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name you have entered in the &quot;attributes&quot; sheet" xr:uid="{00000000-0002-0000-0800-000002000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears on the &quot;attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet.">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears on the &quot;attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet." xr:uid="{00000000-0002-0000-0800-000003000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;" xr:uid="{00000000-0002-0000-0800-000004000000}">
           <x14:formula1>
             <xm:f>Entities!$J$4:$J$30</xm:f>
           </x14:formula1>
           <xm:sqref>B51:B100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000005000000}">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$11</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Auto stash before merge of "main" and "origin/main"
</commit_message>
<xml_diff>
--- a/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
+++ b/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whiteatl\Documents\ble-metadata-template\example_submission_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Data-Notes\BLE-Practices\metadata_templates\canon\example_submission_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDC5227-2B70-4AD0-9E95-1AB1EE4D739F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5256" yWindow="468" windowWidth="25608" windowHeight="14232" tabRatio="913" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -29,7 +28,7 @@
   <externalReferences>
     <externalReference r:id="rId13"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="342">
   <si>
     <t>StorageType</t>
   </si>
@@ -1065,24 +1064,12 @@
   </si>
   <si>
     <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2020GB006552</t>
-  </si>
-  <si>
-    <t>Core Program?</t>
-  </si>
-  <si>
-    <t>Primarily funded by BLE LTER?</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1428,7 +1415,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1740,14 +1727,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1762,7 +1751,7 @@
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="27" t="s">
         <v>194</v>
@@ -1779,7 +1768,7 @@
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="27" t="s">
         <v>193</v>
@@ -1796,7 +1785,7 @@
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -1818,21 +1807,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -1852,21 +1841,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>335</v>
       </c>
@@ -1874,7 +1863,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>341</v>
       </c>
@@ -1884,14 +1873,14 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="info to ID the publication: can be a citation (any format), a DOI, a link" sqref="A1" xr:uid="{00000000-0002-0000-0A00-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="indicate the relationship between the dataset and the publication" sqref="B1" xr:uid="{00000000-0002-0000-0A00-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="info to ID the publication: can be a citation (any format), a DOI, a link" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="indicate the relationship between the dataset and the publication" sqref="B1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lookup_tables!$A$28:$A$30</xm:f>
           </x14:formula1>
@@ -1904,23 +1893,25 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="64.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" customWidth="1"/>
+    <col min="4" max="4" width="44.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="64.5546875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>86</v>
       </c>
@@ -1935,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>54</v>
       </c>
@@ -1958,7 +1949,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
@@ -1981,7 +1972,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>57</v>
       </c>
@@ -2001,7 +1992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
@@ -2021,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>77</v>
       </c>
@@ -2044,7 +2035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>79</v>
       </c>
@@ -2062,7 +2053,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>82</v>
       </c>
@@ -2080,7 +2071,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F9" s="14" t="s">
         <v>94</v>
       </c>
@@ -2088,7 +2079,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -2111,7 +2102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2128,7 +2119,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2145,7 +2136,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2160,7 +2151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2175,7 +2166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
         <v>30</v>
       </c>
@@ -2187,7 +2178,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
@@ -2197,7 +2188,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>6</v>
       </c>
@@ -2207,13 +2198,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
       <c r="I18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>104</v>
       </c>
@@ -2225,7 +2216,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>105</v>
       </c>
@@ -2242,7 +2233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -2259,7 +2250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -2270,7 +2261,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -2281,7 +2272,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2292,7 +2283,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2303,32 +2294,32 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>340</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -2336,35 +2327,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2410,14 +2398,8 @@
       <c r="O1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D2" s="6" t="s">
         <v>195</v>
       </c>
@@ -2446,14 +2428,8 @@
       <c r="O2" t="s">
         <v>334</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2463,32 +2439,26 @@
       <c r="N4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 15 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Send us a Word doc and enter file name here. See PDF for guidelines." sqref="E2:E4 H2:H4" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Earliest date in dataset. Use YYYY-MM-DD or YYYY." sqref="I2:I4" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latest date in dataset. Use YYYY-MM-DD or YYYY." sqref="J2:J4" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CC0 or Creative Commons 0, a public domain license, is the license we use for our datasets. If you wish to use a different license, please discuss with the information managers." sqref="M2:M4" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The timezone used for any date/time values supplied in this dataset." sqref="N2:N4" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Is this a BLE Core Program dataset?" sqref="P2" xr:uid="{45D80D48-DC92-448B-BE8A-5902A4656AE5}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Was this dataset primarly funded by BLE? If not, you'll need to provide the information manager with details about other projects funding this dataset." sqref="Q2" xr:uid="{0053398A-2209-4777-BEC2-C55F217D7B23}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
+  <dataValidations count="6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 15 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Send us a Word doc and enter file name here. See PDF for guidelines." sqref="E2:E4 H2:H4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Earliest date in dataset. Use YYYY-MM-DD or YYYY." sqref="I2:I4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latest date in dataset. Use YYYY-MM-DD or YYYY." sqref="J2:J4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CC0 or Creative Commons 0, a public domain license, is the license we use for our datasets. If you wish to use a different license, please discuss with the information managers." sqref="M2:M4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The timezone used for any date/time values supplied in this dataset." sqref="N2:N4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value." xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value.">
           <x14:formula1>
             <xm:f>lookup_tables!$D$11:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>K2:K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="make sure we can locate this authority" prompt="The taxonomic authority to which you refer when determining taxonomic names in this dataset. The drop-down options are ITIS and WoRMS, commonly used in marine bio, or enter your own." xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="make sure we can locate this authority" prompt="The taxonomic authority to which you refer when determining taxonomic names in this dataset. The drop-down options are ITIS and WoRMS, commonly used in marine bio, or enter your own.">
           <x14:formula1>
             <xm:f>lookup_tables!$D$20:$D$21</xm:f>
           </x14:formula1>
@@ -2501,32 +2471,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
-    <col min="10" max="15" width="8.85546875" style="1"/>
-    <col min="16" max="16" width="8.85546875" style="3"/>
-    <col min="17" max="17" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="13.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="1" customWidth="1"/>
+    <col min="10" max="15" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="8.88671875" style="3"/>
+    <col min="17" max="17" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2591,7 +2561,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2644,30 +2614,30 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" sqref="C1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Number all creators starting with 2." prompt="Analogous to authorship order in a publication. Per LTER best practices, BLE will be first creator to any BLE dataset, so number all creators starting with 2. _x000a__x000a_Leave blank for all other roles." sqref="D3:D4" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" sqref="C1"/>
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Number all creators starting with 2." prompt="Analogous to authorship order in a publication. Per LTER best practices, BLE will be first creator to any BLE dataset, so number all creators starting with 2. _x000a__x000a_Leave blank for all other roles." sqref="D3:D4">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORCID is a unique identifier system for researchers. Sign up at https://orcid.org. This person doesn't have an ORCID? Maybe encourage them to get one and fill out a profile? (Merely having an ORCID is no good without a nice profile.)" sqref="H3:H4" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORCID is a unique identifier system for researchers. Sign up at https://orcid.org. This person doesn't have an ORCID? Maybe encourage them to get one and fill out a profile? (Merely having an ORCID is no good without a nice profile.)" sqref="H3:H4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" xr:uid="{00000000-0002-0000-0200-000003000000}">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list">
           <x14:formula1>
             <xm:f>lookup_tables!$F$3:$F$10</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" prompt="Include dataset creators, but also technicians and other personnel who contribute to and deserve acknowledgment for this dataset._x000a__x000a_Choose from a value in the drop down or enter your own value." xr:uid="{00000000-0002-0000-0200-000004000000}">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" prompt="Include dataset creators, but also technicians and other personnel who contribute to and deserve acknowledgment for this dataset._x000a__x000a_Choose from a value in the drop down or enter your own value.">
           <x14:formula1>
             <xm:f>lookup_tables!$F$3:$F$10</xm:f>
           </x14:formula1>
           <xm:sqref>C3:C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" xr:uid="{00000000-0002-0000-0200-000005000000}">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list">
           <x14:formula1>
             <xm:f>'\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\example_submission_package\[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
           </x14:formula1>
@@ -2680,30 +2650,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="9.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="6"/>
     <col min="7" max="7" width="40" style="6" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="80.28515625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="36.6640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="80.33203125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2729,7 +2699,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>211</v>
       </c>
@@ -2753,7 +2723,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>212</v>
       </c>
@@ -2777,7 +2747,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>213</v>
       </c>
@@ -2801,7 +2771,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>214</v>
       </c>
@@ -2825,7 +2795,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>215</v>
       </c>
@@ -2847,7 +2817,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>216</v>
       </c>
@@ -2869,7 +2839,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>217</v>
       </c>
@@ -2884,7 +2854,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>218</v>
       </c>
@@ -2899,7 +2869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>219</v>
       </c>
@@ -2914,7 +2884,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>220</v>
       </c>
@@ -2929,7 +2899,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>221</v>
       </c>
@@ -2944,7 +2914,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>222</v>
       </c>
@@ -2959,7 +2929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>223</v>
       </c>
@@ -2974,7 +2944,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>224</v>
       </c>
@@ -2989,7 +2959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>225</v>
       </c>
@@ -3004,7 +2974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>226</v>
       </c>
@@ -3019,7 +2989,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>227</v>
       </c>
@@ -3034,7 +3004,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>228</v>
       </c>
@@ -3049,7 +3019,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>229</v>
       </c>
@@ -3064,7 +3034,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>230</v>
       </c>
@@ -3081,34 +3051,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid">
           <x14:formula1>
             <xm:f>lookup_tables!$C$11:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>E22:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lookup_tables!$A$3:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>D5:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="We highly recommend choosing keywords from an existing keyword set, aka thesaurus. See the included table for links to preferred thesauri. _x000a__x000a_Choose from the drop-down menu. Choose &quot;none&quot; if the keyword did not come from any thesauri (not recommended!)." xr:uid="{00000000-0002-0000-0300-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="We highly recommend choosing keywords from an existing keyword set, aka thesaurus. See the included table for links to preferred thesauri. _x000a__x000a_Choose from the drop-down menu. Choose &quot;none&quot; if the keyword did not come from any thesauri (not recommended!).">
           <x14:formula1>
             <xm:f>lookup_tables!$A$3:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid" xr:uid="{00000000-0002-0000-0300-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid">
           <x14:formula1>
             <xm:f>'\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\example_submission_package\[example_metadata-Lougheed.xlsx]lookup_tables'!#REF!</xm:f>
           </x14:formula1>
@@ -3121,7 +3091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3129,27 +3099,27 @@
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="24.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="24.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3202,7 +3172,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>131</v>
       </c>
@@ -3213,29 +3183,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="8" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3267,7 +3237,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2"/>
       <c r="C2" s="6" t="s">
         <v>231</v>
@@ -3286,7 +3256,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3"/>
       <c r="C3" s="6" t="s">
         <v>235</v>
@@ -3305,7 +3275,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C4" s="6" t="s">
         <v>238</v>
       </c>
@@ -3323,7 +3293,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
         <v>241</v>
       </c>
@@ -3343,7 +3313,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
@@ -3352,37 +3322,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="1"/>
+    <col min="17" max="17" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -3435,7 +3405,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -3453,7 +3423,7 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
     </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -3471,7 +3441,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -3489,7 +3459,7 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -3507,7 +3477,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -3525,7 +3495,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -3549,7 +3519,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -3573,7 +3543,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -3591,7 +3561,7 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -3609,7 +3579,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>231</v>
       </c>
@@ -3627,7 +3597,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>231</v>
       </c>
@@ -3651,7 +3621,7 @@
       </c>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>231</v>
       </c>
@@ -3675,7 +3645,7 @@
       </c>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>231</v>
       </c>
@@ -3697,7 +3667,7 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>231</v>
       </c>
@@ -3721,7 +3691,7 @@
       </c>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>231</v>
       </c>
@@ -3745,7 +3715,7 @@
       </c>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>231</v>
       </c>
@@ -3767,7 +3737,7 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" ht="72" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>231</v>
       </c>
@@ -3789,7 +3759,7 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>231</v>
       </c>
@@ -3811,7 +3781,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>231</v>
       </c>
@@ -3829,7 +3799,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>235</v>
       </c>
@@ -3847,7 +3817,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>235</v>
       </c>
@@ -3865,7 +3835,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>235</v>
       </c>
@@ -3889,7 +3859,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>235</v>
       </c>
@@ -3913,7 +3883,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>235</v>
       </c>
@@ -3931,7 +3901,7 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>235</v>
       </c>
@@ -3953,7 +3923,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>235</v>
       </c>
@@ -3977,7 +3947,7 @@
       </c>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>235</v>
       </c>
@@ -3999,7 +3969,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>238</v>
       </c>
@@ -4023,7 +3993,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>238</v>
       </c>
@@ -4047,7 +4017,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>238</v>
       </c>
@@ -4065,7 +4035,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>238</v>
       </c>
@@ -4083,7 +4053,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>238</v>
       </c>
@@ -4101,7 +4071,7 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="2:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>238</v>
       </c>
@@ -4123,7 +4093,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>238</v>
       </c>
@@ -4147,7 +4117,7 @@
       </c>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>238</v>
       </c>
@@ -4169,7 +4139,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>238</v>
       </c>
@@ -4193,7 +4163,7 @@
       </c>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>238</v>
       </c>
@@ -4217,7 +4187,7 @@
       </c>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>241</v>
       </c>
@@ -4241,7 +4211,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>241</v>
       </c>
@@ -4265,7 +4235,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>241</v>
       </c>
@@ -4283,7 +4253,7 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>241</v>
       </c>
@@ -4301,7 +4271,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>241</v>
       </c>
@@ -4325,7 +4295,7 @@
       </c>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" ht="72" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>241</v>
       </c>
@@ -4347,7 +4317,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="2:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>241</v>
       </c>
@@ -4369,27 +4339,27 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter whole numbers numbering your columns" sqref="C101:C1048576" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter whole numbers numbering your columns" sqref="C101:C1048576">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." sqref="C46:C49 C51:C100" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." sqref="C46:C49 C51:C100">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." sqref="N46:N100" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." sqref="N46:N100">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value." sqref="P46:Q100" xr:uid="{00000000-0002-0000-0600-000003000000}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value." sqref="P46:Q100">
       <formula1>ISNUMBER(P45)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value" sqref="N2:N45" xr:uid="{00000000-0002-0000-0600-000004000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value" sqref="N2:N45">
       <formula1>ISNUMBER(N2)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value_x000a_" sqref="P2:Q45" xr:uid="{00000000-0002-0000-0600-000005000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter a numeric value_x000a_" sqref="P2:Q45">
       <formula1>ISNUMBER(P2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -4398,31 +4368,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from the four!" prompt="choose from four number types" xr:uid="{00000000-0002-0000-0600-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from the four!" prompt="choose from four number types">
           <x14:formula1>
             <xm:f>lookup_tables!$A$11:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>O2:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" error="choose from the seven!" prompt="choose from the seven" xr:uid="{00000000-0002-0000-0600-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" error="choose from the seven!" prompt="choose from the seven">
           <x14:formula1>
             <xm:f>lookup_tables!$B$11:$B$17</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I24 I29:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" xr:uid="{00000000-0002-0000-0600-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option">
           <x14:formula1>
             <xm:f>lookup_tables!$I$2:$I$21</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H24 H29:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;" xr:uid="{00000000-0002-0000-0600-000009000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;">
           <x14:formula1>
             <xm:f>Entities!$J$4:$J$30</xm:f>
           </x14:formula1>
           <xm:sqref>B51:B100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$11</xm:f>
           </x14:formula1>
@@ -4435,23 +4405,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4468,7 +4438,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -4482,7 +4452,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -4496,7 +4466,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4510,7 +4480,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -4524,7 +4494,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -4538,7 +4508,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -4552,7 +4522,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -4566,7 +4536,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -4580,7 +4550,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -4594,7 +4564,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>231</v>
       </c>
@@ -4608,7 +4578,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>231</v>
       </c>
@@ -4622,7 +4592,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>231</v>
       </c>
@@ -4638,32 +4608,32 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact code as appears in data." sqref="D2:D4" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Define this code (even if it seems self-explanatory)." sqref="E2:E4" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact code as appears in data." sqref="D2:D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Define this code (even if it seems self-explanatory)." sqref="E2:E4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that you have entered in the &quot;Attributes&quot; sheet" xr:uid="{00000000-0002-0000-0700-000002000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that you have entered in the &quot;Attributes&quot; sheet">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears in the &quot;Attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet." xr:uid="{00000000-0002-0000-0700-000003000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears in the &quot;Attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet.">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B50</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;" xr:uid="{00000000-0002-0000-0700-000005000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;">
           <x14:formula1>
             <xm:f>Entities!$J$4:$J$30</xm:f>
           </x14:formula1>
@@ -4676,25 +4646,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4711,7 +4681,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>231</v>
       </c>
@@ -4725,7 +4695,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>231</v>
       </c>
@@ -4739,7 +4709,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>231</v>
       </c>
@@ -4753,7 +4723,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>231</v>
       </c>
@@ -4767,7 +4737,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
@@ -4781,7 +4751,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
@@ -4795,7 +4765,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
@@ -4809,7 +4779,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>231</v>
       </c>
@@ -4823,7 +4793,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>231</v>
       </c>
@@ -4837,7 +4807,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>235</v>
       </c>
@@ -4851,7 +4821,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>235</v>
       </c>
@@ -4865,7 +4835,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>235</v>
       </c>
@@ -4879,7 +4849,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>235</v>
       </c>
@@ -4893,7 +4863,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>235</v>
       </c>
@@ -4907,7 +4877,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>235</v>
       </c>
@@ -4921,7 +4891,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>238</v>
       </c>
@@ -4935,7 +4905,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>238</v>
       </c>
@@ -4949,7 +4919,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>238</v>
       </c>
@@ -4963,7 +4933,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>238</v>
       </c>
@@ -4977,7 +4947,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>241</v>
       </c>
@@ -4991,7 +4961,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>241</v>
       </c>
@@ -5007,32 +4977,32 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact missing value code as appears in data." sqref="D2:D4" xr:uid="{00000000-0002-0000-0800-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Why are missing values represented by this code missing? " sqref="E2:E4" xr:uid="{00000000-0002-0000-0800-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact missing value code as appears in data." sqref="D2:D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Why are missing values represented by this code missing? " sqref="E2:E4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name you have entered in the &quot;attributes&quot; sheet" xr:uid="{00000000-0002-0000-0800-000002000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name you have entered in the &quot;attributes&quot; sheet">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears on the &quot;attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet." xr:uid="{00000000-0002-0000-0800-000003000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears on the &quot;attributes&quot; sheet" prompt="Where does this code appears? The drop-down options correspond to entries in &quot;Attributes&quot; sheet.">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;" xr:uid="{00000000-0002-0000-0800-000004000000}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a valid file or worksheet name as entered in &quot;Entities&quot;">
           <x14:formula1>
             <xm:f>Entities!$J$4:$J$30</xm:f>
           </x14:formula1>
           <xm:sqref>B51:B100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$11</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Git seemed to lose track of binary file status. Nothing changed.
Committing just to make git think the repo is current.
</commit_message>
<xml_diff>
--- a/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
+++ b/example_submission_package/Lougheed-Completed-Metadata-Example.xlsx
@@ -5012,4 +5012,210 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100882C529237D29E4FB56CB817054A65E4" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11007fc7b13632b201018663e88df6d3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c907e88d-5302-4b6f-a5b9-b4c8999f2445" xmlns:ns3="44f1a407-ca9e-4dc1-a70d-db0c5e3d43f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34701c46d73951006dead7ee579c1c1a" ns2:_="" ns3:_="">
+    <xsd:import namespace="c907e88d-5302-4b6f-a5b9-b4c8999f2445"/>
+    <xsd:import namespace="44f1a407-ca9e-4dc1-a70d-db0c5e3d43f7"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c907e88d-5302-4b6f-a5b9-b4c8999f2445" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="08c7800f-3133-4166-986f-ae8bcd499822" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="44f1a407-ca9e-4dc1-a70d-db0c5e3d43f7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{3ad7614f-57e2-434e-ad01-543da0eb732a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="44f1a407-ca9e-4dc1-a70d-db0c5e3d43f7">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{019FCB57-F3EF-412C-949C-878710631B89}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{329F7B65-10D7-4E2C-8BF6-93450AC660E5}"/>
 </file>
</xml_diff>